<commit_message>
Added tRNA shuffling project code
</commit_message>
<xml_diff>
--- a/calculations/maxPackData.xlsx
+++ b/calculations/maxPackData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Documents/TranslationDynamics/calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABF84E7-7883-DD49-9298-11A9A1B22224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C467F1F7-A5B6-4B42-9A7C-20DBAC81B853}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14380" yWindow="2940" windowWidth="25240" windowHeight="13940" xr2:uid="{C68AE7B0-C6D8-CF4F-B2FE-DB2F45F51842}"/>
+    <workbookView xWindow="13540" yWindow="1860" windowWidth="25240" windowHeight="13940" xr2:uid="{C68AE7B0-C6D8-CF4F-B2FE-DB2F45F51842}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -557,13 +557,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -575,13 +575,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -898,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3DD95F-89FB-AF4B-AD5D-9A961DE2C5EF}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,7 +977,7 @@
         <v>0.76</v>
       </c>
       <c r="G3" s="29">
-        <f t="shared" ref="G3:G12" si="0">F3*0.9</f>
+        <f t="shared" ref="G3:G21" si="0">F3*0.9</f>
         <v>0.68400000000000005</v>
       </c>
     </row>
@@ -1127,75 +1127,275 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>6</v>
+        <v>4.5</v>
       </c>
       <c r="B10" s="31">
-        <v>0.27616034407233497</v>
+        <v>0.25545089444126301</v>
       </c>
       <c r="C10" s="31">
-        <v>0.24375029640447199</v>
+        <v>0.178903315172766</v>
       </c>
       <c r="D10" s="31">
-        <v>6.9015756027817801E-2</v>
+        <v>8.1587169045470601E-2</v>
       </c>
       <c r="E10" s="31">
-        <v>0.58892639650462497</v>
+        <v>0.51594137865949896</v>
       </c>
       <c r="F10" s="29">
-        <v>0.78</v>
+        <v>0.79700000000000004</v>
       </c>
       <c r="G10" s="29">
         <f t="shared" si="0"/>
-        <v>0.70200000000000007</v>
+        <v>0.71730000000000005</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="31">
-        <v>0.29274438595603097</v>
+        <v>0.26353599087589802</v>
       </c>
       <c r="C11" s="31">
-        <v>0.33206461447458202</v>
+        <v>0.20032595499306999</v>
       </c>
       <c r="D11" s="31">
-        <v>5.2745426198961401E-2</v>
+        <v>7.7406968979675597E-2</v>
       </c>
       <c r="E11" s="31">
-        <v>0.67755442662957399</v>
+        <v>0.54126891484864403</v>
       </c>
       <c r="F11" s="29">
-        <v>0.75</v>
+        <v>0.79200000000000004</v>
       </c>
       <c r="G11" s="29">
-        <f>F11*0.9</f>
-        <v>0.67500000000000004</v>
+        <f t="shared" si="0"/>
+        <v>0.7128000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>10</v>
+        <v>5.5</v>
       </c>
       <c r="B12" s="31">
+        <v>0.27034870497165597</v>
+      </c>
+      <c r="C12" s="31">
+        <v>0.22195534252704499</v>
+      </c>
+      <c r="D12" s="31">
+        <v>7.3203772638913298E-2</v>
+      </c>
+      <c r="E12" s="31">
+        <v>0.56550782013761502</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G12" s="29">
+        <f t="shared" si="0"/>
+        <v>0.70650000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="31">
+        <v>0.27616034407233497</v>
+      </c>
+      <c r="C13" s="31">
+        <v>0.24375029640447199</v>
+      </c>
+      <c r="D13" s="31">
+        <v>6.9015756027817801E-2</v>
+      </c>
+      <c r="E13" s="31">
+        <v>0.58892639650462497</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="G13" s="29">
+        <f t="shared" si="0"/>
+        <v>0.70020000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>6.5</v>
+      </c>
+      <c r="B14" s="31">
+        <v>0.281171327964644</v>
+      </c>
+      <c r="C14" s="31">
+        <v>0.26567989133257802</v>
+      </c>
+      <c r="D14" s="31">
+        <v>6.4865562005799501E-2</v>
+      </c>
+      <c r="E14" s="31">
+        <v>0.61171678130302198</v>
+      </c>
+      <c r="F14" s="29">
+        <v>0.77</v>
+      </c>
+      <c r="G14" s="29">
+        <f t="shared" si="0"/>
+        <v>0.69300000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15" s="31">
+        <v>0.28553270069366099</v>
+      </c>
+      <c r="C15" s="31">
+        <v>0.28772045243288003</v>
+      </c>
+      <c r="D15" s="31">
+        <v>6.0766298079378098E-2</v>
+      </c>
+      <c r="E15" s="31">
+        <v>0.63401945120591896</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0.76</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.68400000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>7.5</v>
+      </c>
+      <c r="B16" s="31">
+        <v>0.28936030773535398</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0.30985354806780202</v>
+      </c>
+      <c r="D16" s="31">
+        <v>5.6725119372691202E-2</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.65593897517584798</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0.752</v>
+      </c>
+      <c r="G16" s="29">
+        <f t="shared" si="0"/>
+        <v>0.67680000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" s="31">
         <v>0.29274438595603097</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C17" s="31">
         <v>0.33206461447458202</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D17" s="31">
         <v>5.2745426198961401E-2</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E17" s="31">
         <v>0.67755442662957399</v>
       </c>
-      <c r="F12" s="29">
-        <v>0.72</v>
-      </c>
-      <c r="G12" s="29">
-        <f>F12*0.9</f>
-        <v>0.64800000000000002</v>
-      </c>
+      <c r="F17" s="29">
+        <v>0.747</v>
+      </c>
+      <c r="G17" s="29">
+        <f t="shared" si="0"/>
+        <v>0.67230000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>8.5</v>
+      </c>
+      <c r="B18" s="31">
+        <v>0.29575620124149399</v>
+      </c>
+      <c r="C18" s="31">
+        <v>0.354341991749136</v>
+      </c>
+      <c r="D18" s="31">
+        <v>4.8828241280727998E-2</v>
+      </c>
+      <c r="E18" s="31">
+        <v>0.69892643427135803</v>
+      </c>
+      <c r="F18" s="29">
+        <v>0.74</v>
+      </c>
+      <c r="G18" s="29">
+        <f t="shared" si="0"/>
+        <v>0.66600000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" s="31">
+        <v>0.29845273731297001</v>
+      </c>
+      <c r="C19" s="31">
+        <v>0.37667623446202098</v>
+      </c>
+      <c r="D19" s="31">
+        <v>4.4973087985010901E-2</v>
+      </c>
+      <c r="E19" s="31">
+        <v>0.72010205976000197</v>
+      </c>
+      <c r="F19" s="29">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="G19" s="29">
+        <f t="shared" si="0"/>
+        <v>0.66149999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>9.5</v>
+      </c>
+      <c r="B20" s="31">
+        <v>0.30088006885044</v>
+      </c>
+      <c r="C20" s="31">
+        <v>0.39905960976618599</v>
+      </c>
+      <c r="D20" s="31">
+        <v>4.1178558015569702E-2</v>
+      </c>
+      <c r="E20" s="31">
+        <v>0.741118236632196</v>
+      </c>
+      <c r="F20" s="29">
+        <v>0.73</v>
+      </c>
+      <c r="G20" s="29">
+        <f t="shared" si="0"/>
+        <v>0.65700000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1261,7 +1461,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="33">
+      <c r="A2" s="39">
         <v>-1</v>
       </c>
       <c r="B2" s="36">
@@ -1273,7 +1473,7 @@
       <c r="D2" s="36">
         <v>-1</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="33">
         <v>-1</v>
       </c>
       <c r="F2" s="26">
@@ -1308,11 +1508,11 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="34"/>
+      <c r="A3" s="40"/>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="37"/>
-      <c r="E3" s="40"/>
+      <c r="E3" s="34"/>
       <c r="F3" s="27">
         <v>6</v>
       </c>
@@ -1345,11 +1545,11 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
-      <c r="E4" s="41"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="28">
         <v>8</v>
       </c>
@@ -1382,7 +1582,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="33">
+      <c r="A5" s="39">
         <v>-1</v>
       </c>
       <c r="B5" s="36">
@@ -1394,7 +1594,7 @@
       <c r="D5" s="36">
         <v>-1</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="33">
         <v>0</v>
       </c>
       <c r="F5" s="26">
@@ -1421,7 +1621,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="34">
+      <c r="A6" s="40">
         <v>-1</v>
       </c>
       <c r="B6" s="37">
@@ -1433,7 +1633,7 @@
       <c r="D6" s="37">
         <v>-1</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="34">
         <v>0</v>
       </c>
       <c r="F6" s="27">
@@ -1460,7 +1660,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35">
+      <c r="A7" s="41">
         <v>-1</v>
       </c>
       <c r="B7" s="38">
@@ -1472,7 +1672,7 @@
       <c r="D7" s="38">
         <v>-1</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="35">
         <v>0</v>
       </c>
       <c r="F7" s="28">
@@ -1499,7 +1699,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="33">
+      <c r="A8" s="39">
         <v>-1</v>
       </c>
       <c r="B8" s="36">
@@ -1511,7 +1711,7 @@
       <c r="D8" s="36">
         <v>0</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="33">
         <v>-1</v>
       </c>
       <c r="F8" s="26">
@@ -1538,7 +1738,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="34">
+      <c r="A9" s="40">
         <v>-1</v>
       </c>
       <c r="B9" s="37">
@@ -1550,7 +1750,7 @@
       <c r="D9" s="37">
         <v>0</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="34">
         <v>-1</v>
       </c>
       <c r="F9" s="27">
@@ -1577,7 +1777,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
+      <c r="A10" s="41">
         <v>-1</v>
       </c>
       <c r="B10" s="38">
@@ -1589,7 +1789,7 @@
       <c r="D10" s="38">
         <v>0</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="35">
         <v>-1</v>
       </c>
       <c r="F10" s="28">
@@ -1616,7 +1816,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="33">
+      <c r="A11" s="39">
         <v>-1</v>
       </c>
       <c r="B11" s="36">
@@ -1628,7 +1828,7 @@
       <c r="D11" s="36">
         <v>-1</v>
       </c>
-      <c r="E11" s="39">
+      <c r="E11" s="33">
         <v>-1</v>
       </c>
       <c r="F11" s="26">
@@ -1655,7 +1855,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="34">
+      <c r="A12" s="40">
         <v>-1</v>
       </c>
       <c r="B12" s="37">
@@ -1667,7 +1867,7 @@
       <c r="D12" s="37">
         <v>-1</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="34">
         <v>-1</v>
       </c>
       <c r="F12" s="27">
@@ -1694,7 +1894,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
+      <c r="A13" s="41">
         <v>-1</v>
       </c>
       <c r="B13" s="38">
@@ -1706,7 +1906,7 @@
       <c r="D13" s="38">
         <v>-1</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="35">
         <v>-1</v>
       </c>
       <c r="F13" s="28">
@@ -1733,7 +1933,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="33">
+      <c r="A14" s="39">
         <v>-1</v>
       </c>
       <c r="B14" s="36">
@@ -1745,7 +1945,7 @@
       <c r="D14" s="36">
         <v>-1</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="33">
         <v>-1</v>
       </c>
       <c r="F14" s="26">
@@ -1772,7 +1972,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="34">
+      <c r="A15" s="40">
         <v>-1</v>
       </c>
       <c r="B15" s="37">
@@ -1784,7 +1984,7 @@
       <c r="D15" s="37">
         <v>-1</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="34">
         <v>-1</v>
       </c>
       <c r="F15" s="27">
@@ -1811,7 +2011,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35">
+      <c r="A16" s="41">
         <v>-1</v>
       </c>
       <c r="B16" s="38">
@@ -1823,7 +2023,7 @@
       <c r="D16" s="38">
         <v>-1</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="35">
         <v>-1</v>
       </c>
       <c r="F16" s="28">
@@ -1850,7 +2050,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="33">
+      <c r="A17" s="39">
         <v>-1</v>
       </c>
       <c r="B17" s="36">
@@ -1862,7 +2062,7 @@
       <c r="D17" s="36">
         <v>0</v>
       </c>
-      <c r="E17" s="39">
+      <c r="E17" s="33">
         <v>0</v>
       </c>
       <c r="F17" s="26">
@@ -1889,7 +2089,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="34">
+      <c r="A18" s="40">
         <v>-1</v>
       </c>
       <c r="B18" s="37">
@@ -1901,7 +2101,7 @@
       <c r="D18" s="37">
         <v>0</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="34">
         <v>0</v>
       </c>
       <c r="F18" s="27">
@@ -1928,7 +2128,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35">
+      <c r="A19" s="41">
         <v>-1</v>
       </c>
       <c r="B19" s="38">
@@ -1940,7 +2140,7 @@
       <c r="D19" s="38">
         <v>0</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="35">
         <v>0</v>
       </c>
       <c r="F19" s="28">
@@ -1967,7 +2167,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="33">
+      <c r="A20" s="39">
         <v>-1</v>
       </c>
       <c r="B20" s="36">
@@ -1979,7 +2179,7 @@
       <c r="D20" s="36">
         <v>-1</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="33">
         <v>0</v>
       </c>
       <c r="F20" s="26">
@@ -2006,7 +2206,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="34">
+      <c r="A21" s="40">
         <v>-1</v>
       </c>
       <c r="B21" s="37">
@@ -2018,7 +2218,7 @@
       <c r="D21" s="37">
         <v>-1</v>
       </c>
-      <c r="E21" s="40">
+      <c r="E21" s="34">
         <v>0</v>
       </c>
       <c r="F21" s="27">
@@ -2045,7 +2245,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35">
+      <c r="A22" s="41">
         <v>-1</v>
       </c>
       <c r="B22" s="38">
@@ -2057,7 +2257,7 @@
       <c r="D22" s="38">
         <v>-1</v>
       </c>
-      <c r="E22" s="41">
+      <c r="E22" s="35">
         <v>0</v>
       </c>
       <c r="F22" s="28">
@@ -2084,7 +2284,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="33">
+      <c r="A23" s="39">
         <v>-1</v>
       </c>
       <c r="B23" s="36">
@@ -2096,7 +2296,7 @@
       <c r="D23" s="36">
         <v>0</v>
       </c>
-      <c r="E23" s="39">
+      <c r="E23" s="33">
         <v>0</v>
       </c>
       <c r="F23" s="26">
@@ -2123,7 +2323,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="34">
+      <c r="A24" s="40">
         <v>-1</v>
       </c>
       <c r="B24" s="37">
@@ -2135,7 +2335,7 @@
       <c r="D24" s="37">
         <v>0</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="34">
         <v>0</v>
       </c>
       <c r="F24" s="27">
@@ -2162,7 +2362,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35">
+      <c r="A25" s="41">
         <v>-1</v>
       </c>
       <c r="B25" s="38">
@@ -2174,7 +2374,7 @@
       <c r="D25" s="38">
         <v>0</v>
       </c>
-      <c r="E25" s="41">
+      <c r="E25" s="35">
         <v>0</v>
       </c>
       <c r="F25" s="28">
@@ -2201,7 +2401,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="33">
+      <c r="A26" s="39">
         <v>0</v>
       </c>
       <c r="B26" s="36">
@@ -2213,7 +2413,7 @@
       <c r="D26" s="36">
         <v>0</v>
       </c>
-      <c r="E26" s="39">
+      <c r="E26" s="33">
         <v>0</v>
       </c>
       <c r="F26" s="26">
@@ -2240,7 +2440,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="34">
+      <c r="A27" s="40">
         <v>0</v>
       </c>
       <c r="B27" s="37">
@@ -2252,7 +2452,7 @@
       <c r="D27" s="37">
         <v>0</v>
       </c>
-      <c r="E27" s="40">
+      <c r="E27" s="34">
         <v>0</v>
       </c>
       <c r="F27" s="27">
@@ -2279,7 +2479,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35">
+      <c r="A28" s="41">
         <v>0</v>
       </c>
       <c r="B28" s="38">
@@ -2291,7 +2491,7 @@
       <c r="D28" s="38">
         <v>0</v>
       </c>
-      <c r="E28" s="41">
+      <c r="E28" s="35">
         <v>0</v>
       </c>
       <c r="F28" s="28">
@@ -2318,7 +2518,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="33">
+      <c r="A29" s="39">
         <v>0</v>
       </c>
       <c r="B29" s="36">
@@ -2330,7 +2530,7 @@
       <c r="D29" s="36">
         <v>0</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="33">
         <v>0</v>
       </c>
       <c r="F29" s="26">
@@ -2357,7 +2557,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="34">
+      <c r="A30" s="40">
         <v>0</v>
       </c>
       <c r="B30" s="37">
@@ -2369,7 +2569,7 @@
       <c r="D30" s="37">
         <v>0</v>
       </c>
-      <c r="E30" s="40">
+      <c r="E30" s="34">
         <v>0</v>
       </c>
       <c r="F30" s="27">
@@ -2396,7 +2596,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35">
+      <c r="A31" s="41">
         <v>0</v>
       </c>
       <c r="B31" s="38">
@@ -2408,7 +2608,7 @@
       <c r="D31" s="38">
         <v>0</v>
       </c>
-      <c r="E31" s="41">
+      <c r="E31" s="35">
         <v>0</v>
       </c>
       <c r="F31" s="28">
@@ -2435,7 +2635,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="33">
+      <c r="A32" s="39">
         <v>0</v>
       </c>
       <c r="B32" s="36">
@@ -2447,7 +2647,7 @@
       <c r="D32" s="36">
         <v>0</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="33">
         <v>0</v>
       </c>
       <c r="F32" s="26">
@@ -2474,7 +2674,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="34">
+      <c r="A33" s="40">
         <v>0</v>
       </c>
       <c r="B33" s="37">
@@ -2486,7 +2686,7 @@
       <c r="D33" s="37">
         <v>0</v>
       </c>
-      <c r="E33" s="40">
+      <c r="E33" s="34">
         <v>0</v>
       </c>
       <c r="F33" s="27">
@@ -2513,7 +2713,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35">
+      <c r="A34" s="41">
         <v>0</v>
       </c>
       <c r="B34" s="38">
@@ -2525,7 +2725,7 @@
       <c r="D34" s="38">
         <v>0</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="35">
         <v>0</v>
       </c>
       <c r="F34" s="28">
@@ -2552,7 +2752,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="33">
+      <c r="A35" s="39">
         <v>0</v>
       </c>
       <c r="B35" s="36">
@@ -2564,7 +2764,7 @@
       <c r="D35" s="36">
         <v>-1</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="33">
         <v>0</v>
       </c>
       <c r="F35" s="26">
@@ -2591,7 +2791,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="34">
+      <c r="A36" s="40">
         <v>0</v>
       </c>
       <c r="B36" s="37">
@@ -2603,7 +2803,7 @@
       <c r="D36" s="37">
         <v>-1</v>
       </c>
-      <c r="E36" s="40">
+      <c r="E36" s="34">
         <v>0</v>
       </c>
       <c r="F36" s="27">
@@ -2630,7 +2830,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35">
+      <c r="A37" s="41">
         <v>0</v>
       </c>
       <c r="B37" s="38">
@@ -2642,7 +2842,7 @@
       <c r="D37" s="38">
         <v>-1</v>
       </c>
-      <c r="E37" s="41">
+      <c r="E37" s="35">
         <v>0</v>
       </c>
       <c r="F37" s="28">
@@ -2669,7 +2869,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="33">
+      <c r="A38" s="39">
         <v>0</v>
       </c>
       <c r="B38" s="36">
@@ -2681,7 +2881,7 @@
       <c r="D38" s="36">
         <v>0</v>
       </c>
-      <c r="E38" s="39">
+      <c r="E38" s="33">
         <v>0</v>
       </c>
       <c r="F38" s="26">
@@ -2708,7 +2908,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="34">
+      <c r="A39" s="40">
         <v>0</v>
       </c>
       <c r="B39" s="37">
@@ -2720,7 +2920,7 @@
       <c r="D39" s="37">
         <v>0</v>
       </c>
-      <c r="E39" s="40">
+      <c r="E39" s="34">
         <v>0</v>
       </c>
       <c r="F39" s="27">
@@ -2747,7 +2947,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35">
+      <c r="A40" s="41">
         <v>0</v>
       </c>
       <c r="B40" s="38">
@@ -2759,7 +2959,7 @@
       <c r="D40" s="38">
         <v>0</v>
       </c>
-      <c r="E40" s="41">
+      <c r="E40" s="35">
         <v>0</v>
       </c>
       <c r="F40" s="28">
@@ -2787,11 +2987,56 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="A11:A13"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="A8:A10"/>
@@ -2802,56 +3047,11 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="A38:A40"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A2:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>